<commit_message>
adjusted rec selectivity and test regulation data
I corrected errors in both datasets. The "*_test" should be used when testing the projection model. It contains 2019 regulations.
</commit_message>
<xml_diff>
--- a/directed_trips_regions_bimonthly_test.xlsx
+++ b/directed_trips_regions_bimonthly_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.carr-harris\Dropbox\NMFS\fluke_mse\simulation_R_code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.carr-harris\Desktop\Git\Rec.-deman-modelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109:F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1599,7 +1599,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G14" s="1">
         <v>100</v>
@@ -1685,7 +1685,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G15" s="1">
         <v>100</v>
@@ -1771,7 +1771,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G16" s="1">
         <v>100</v>
@@ -1857,7 +1857,7 @@
         <v>4</v>
       </c>
       <c r="F17" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G17" s="1">
         <v>100</v>
@@ -1943,7 +1943,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G18" s="1">
         <v>100</v>
@@ -2029,7 +2029,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G19" s="1">
         <v>100</v>
@@ -2115,7 +2115,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G20" s="1">
         <v>100</v>
@@ -2201,7 +2201,7 @@
         <v>4</v>
       </c>
       <c r="F21" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G21" s="1">
         <v>100</v>
@@ -2287,7 +2287,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G22" s="1">
         <v>100</v>
@@ -2373,7 +2373,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G23" s="1">
         <v>100</v>
@@ -2459,7 +2459,7 @@
         <v>4</v>
       </c>
       <c r="F24" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G24" s="1">
         <v>100</v>
@@ -2545,7 +2545,7 @@
         <v>4</v>
       </c>
       <c r="F25" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G25" s="1">
         <v>100</v>
@@ -2631,7 +2631,7 @@
         <v>4</v>
       </c>
       <c r="F26" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G26" s="1">
         <v>100</v>
@@ -2717,7 +2717,7 @@
         <v>4</v>
       </c>
       <c r="F27" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G27" s="1">
         <v>100</v>
@@ -2803,7 +2803,7 @@
         <v>4</v>
       </c>
       <c r="F28" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G28" s="1">
         <v>100</v>
@@ -2889,7 +2889,7 @@
         <v>4</v>
       </c>
       <c r="F29" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G29" s="1">
         <v>100</v>
@@ -3921,7 +3921,7 @@
         <v>4</v>
       </c>
       <c r="F41" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G41" s="1">
         <v>100</v>
@@ -4007,7 +4007,7 @@
         <v>4</v>
       </c>
       <c r="F42" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G42" s="1">
         <v>100</v>
@@ -4093,7 +4093,7 @@
         <v>4</v>
       </c>
       <c r="F43" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G43" s="1">
         <v>100</v>
@@ -4179,7 +4179,7 @@
         <v>4</v>
       </c>
       <c r="F44" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G44" s="1">
         <v>100</v>
@@ -4265,7 +4265,7 @@
         <v>4</v>
       </c>
       <c r="F45" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G45" s="1">
         <v>100</v>
@@ -4351,7 +4351,7 @@
         <v>4</v>
       </c>
       <c r="F46" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G46" s="1">
         <v>100</v>
@@ -4437,7 +4437,7 @@
         <v>4</v>
       </c>
       <c r="F47" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G47" s="1">
         <v>100</v>
@@ -4523,7 +4523,7 @@
         <v>4</v>
       </c>
       <c r="F48" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G48" s="1">
         <v>100</v>
@@ -4609,7 +4609,7 @@
         <v>4</v>
       </c>
       <c r="F49" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G49" s="1">
         <v>100</v>
@@ -4695,7 +4695,7 @@
         <v>4</v>
       </c>
       <c r="F50" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G50" s="1">
         <v>100</v>
@@ -4781,7 +4781,7 @@
         <v>4</v>
       </c>
       <c r="F51" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G51" s="1">
         <v>100</v>
@@ -4867,7 +4867,7 @@
         <v>4</v>
       </c>
       <c r="F52" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G52" s="1">
         <v>100</v>
@@ -4953,7 +4953,7 @@
         <v>4</v>
       </c>
       <c r="F53" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G53" s="1">
         <v>100</v>
@@ -5039,7 +5039,7 @@
         <v>4</v>
       </c>
       <c r="F54" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G54" s="1">
         <v>100</v>
@@ -5125,7 +5125,7 @@
         <v>4</v>
       </c>
       <c r="F55" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G55" s="1">
         <v>100</v>
@@ -5211,7 +5211,7 @@
         <v>4</v>
       </c>
       <c r="F56" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="G56" s="1">
         <v>100</v>
@@ -5247,7 +5247,7 @@
         <v>4</v>
       </c>
       <c r="R56" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="S56" s="1">
         <v>100</v>
@@ -5297,7 +5297,7 @@
         <v>4</v>
       </c>
       <c r="F57" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="G57" s="1">
         <v>100</v>
@@ -5333,7 +5333,7 @@
         <v>4</v>
       </c>
       <c r="R57" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="S57" s="1">
         <v>100</v>
@@ -5383,7 +5383,7 @@
         <v>4</v>
       </c>
       <c r="F58" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="G58" s="1">
         <v>100</v>
@@ -5419,7 +5419,7 @@
         <v>4</v>
       </c>
       <c r="R58" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="S58" s="1">
         <v>100</v>
@@ -5469,7 +5469,7 @@
         <v>4</v>
       </c>
       <c r="F59" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="G59" s="1">
         <v>100</v>
@@ -5505,7 +5505,7 @@
         <v>4</v>
       </c>
       <c r="R59" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="S59" s="1">
         <v>100</v>
@@ -5555,7 +5555,7 @@
         <v>4</v>
       </c>
       <c r="F60" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="G60" s="1">
         <v>100</v>
@@ -5591,7 +5591,7 @@
         <v>4</v>
       </c>
       <c r="R60" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="S60" s="1">
         <v>100</v>
@@ -5641,7 +5641,7 @@
         <v>4</v>
       </c>
       <c r="F61" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="G61" s="1">
         <v>100</v>
@@ -5677,7 +5677,7 @@
         <v>4</v>
       </c>
       <c r="R61" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="S61" s="1">
         <v>100</v>
@@ -5727,7 +5727,7 @@
         <v>4</v>
       </c>
       <c r="F62" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="G62" s="1">
         <v>100</v>
@@ -5763,7 +5763,7 @@
         <v>4</v>
       </c>
       <c r="R62" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="S62" s="1">
         <v>100</v>
@@ -5813,7 +5813,7 @@
         <v>4</v>
       </c>
       <c r="F63" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="G63" s="1">
         <v>100</v>
@@ -5849,7 +5849,7 @@
         <v>4</v>
       </c>
       <c r="R63" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="S63" s="1">
         <v>100</v>
@@ -5899,7 +5899,7 @@
         <v>4</v>
       </c>
       <c r="F64" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="G64" s="1">
         <v>100</v>
@@ -5935,7 +5935,7 @@
         <v>4</v>
       </c>
       <c r="R64" s="1">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="S64" s="1">
         <v>100</v>
@@ -9769,7 +9769,7 @@
         <v>4</v>
       </c>
       <c r="F109" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G109" s="1">
         <v>100</v>
@@ -9855,7 +9855,7 @@
         <v>4</v>
       </c>
       <c r="F110" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G110" s="1">
         <v>100</v>
@@ -9941,7 +9941,7 @@
         <v>4</v>
       </c>
       <c r="F111" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G111" s="1">
         <v>100</v>
@@ -10027,7 +10027,7 @@
         <v>4</v>
       </c>
       <c r="F112" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G112" s="1">
         <v>100</v>
@@ -10113,7 +10113,7 @@
         <v>4</v>
       </c>
       <c r="F113" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G113" s="1">
         <v>100</v>
@@ -10199,7 +10199,7 @@
         <v>4</v>
       </c>
       <c r="F114" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G114" s="1">
         <v>100</v>
@@ -10285,7 +10285,7 @@
         <v>4</v>
       </c>
       <c r="F115" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G115" s="1">
         <v>100</v>
@@ -10371,7 +10371,7 @@
         <v>4</v>
       </c>
       <c r="F116" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G116" s="1">
         <v>100</v>
@@ -10457,7 +10457,7 @@
         <v>4</v>
       </c>
       <c r="F117" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G117" s="1">
         <v>100</v>
@@ -10543,7 +10543,7 @@
         <v>4</v>
       </c>
       <c r="F118" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G118" s="1">
         <v>100</v>
@@ -10629,7 +10629,7 @@
         <v>4</v>
       </c>
       <c r="F119" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G119" s="1">
         <v>100</v>
@@ -10715,7 +10715,7 @@
         <v>4</v>
       </c>
       <c r="F120" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G120" s="1">
         <v>100</v>
@@ -10801,7 +10801,7 @@
         <v>4</v>
       </c>
       <c r="F121" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G121" s="1">
         <v>100</v>
@@ -10887,7 +10887,7 @@
         <v>4</v>
       </c>
       <c r="F122" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G122" s="1">
         <v>100</v>
@@ -10973,7 +10973,7 @@
         <v>4</v>
       </c>
       <c r="F123" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G123" s="1">
         <v>100</v>
@@ -11059,7 +11059,7 @@
         <v>4</v>
       </c>
       <c r="F124" s="1">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="G124" s="1">
         <v>100</v>

</xml_diff>